<commit_message>
excel write and read config
</commit_message>
<xml_diff>
--- a/Testdata.xlsx
+++ b/Testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\VimanNagar\May 21\16 April Selenium Basics\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Username1</t>
   </si>
@@ -141,12 +141,22 @@
   </si>
   <si>
     <t>Password20</t>
+  </si>
+  <si>
+    <t>testvalue</t>
+  </si>
+  <si>
+    <t>new row and new column test</t>
+  </si>
+  <si>
+    <t>existing row and new column</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,7 +468,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
@@ -466,8 +476,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -520,7 +530,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>56</v>
@@ -597,6 +607,9 @@
       <c r="B16" t="s">
         <v>34</v>
       </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -628,6 +641,11 @@
       </c>
       <c r="B20" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="N51" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>